<commit_message>
Update results and plots
</commit_message>
<xml_diff>
--- a/plots/Ergebnisse_Überblick.xlsx
+++ b/plots/Ergebnisse_Überblick.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willi\Desktop\Sound-Event-Detection\plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ADEA261-428F-444D-B1BF-2C1A2ED49749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCBABF6-CDDC-47F5-AB4E-0BA0CB061214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{2C3619C7-81E7-49C3-8410-F5775DF0AEF0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>AdvancedCRNN</t>
   </si>
@@ -177,6 +177,27 @@
   </si>
   <si>
     <t>0.2286</t>
+  </si>
+  <si>
+    <t>Binary Bird Dataset</t>
+  </si>
+  <si>
+    <t>0.4154</t>
+  </si>
+  <si>
+    <t>0.5869</t>
+  </si>
+  <si>
+    <t>0.8834</t>
+  </si>
+  <si>
+    <t>0.8493</t>
+  </si>
+  <si>
+    <t>0.9163</t>
+  </si>
+  <si>
+    <t>0.7915</t>
   </si>
 </sst>
 </file>
@@ -220,10 +241,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D178EF0-4385-470A-802A-049C10FFDC17}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,9 +591,10 @@
     <col min="4" max="4" width="7.42578125" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -586,8 +607,11 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
@@ -601,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -623,8 +647,11 @@
       <c r="H3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -643,8 +670,11 @@
       <c r="H4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
@@ -663,8 +693,11 @@
       <c r="H5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -683,8 +716,11 @@
       <c r="H6" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,8 +742,11 @@
       <c r="H8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -726,8 +765,11 @@
       <c r="H9" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -746,8 +788,11 @@
       <c r="H10" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -763,8 +808,11 @@
       <c r="F11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>44</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>